<commit_message>
added the new excel
</commit_message>
<xml_diff>
--- a/phonics_lessons.xlsx
+++ b/phonics_lessons.xlsx
@@ -7,7 +7,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -871,13 +871,13 @@
     <t xml:space="preserve">zap, zip, quiz, zen, zest,zit </t>
   </si>
   <si>
-    <t>at, as, map, sad, sat, had, has, bad, and, an, can, pan, hand, plant, plan, lamp</t>
-  </si>
-  <si>
-    <t>if, it, him, win, big, sit, did, hit, sits, list, skin, twin, flip, trip</t>
-  </si>
-  <si>
-    <t>on, mom, lot, hot, fox, job, spot, stop, frog, loss, pond, soft</t>
+    <t xml:space="preserve">at, as, map, sad, sat, had, has, bad, and, an, can, pan, hand, plant, plan, lamp, hat, mat, gap, dad, tag, gas, mad, jab, ax, nab, dab, tap, lab, cat,  zap, fat, map,  ban, van, ram, man, jam, tan, fan, man, ham, fast, grab, crab, band, clap, slab, slam, scan, mask, pact, rasp, sand, raft, flag, pant, vast, flap, past, last, damp, cast, slapm, flap</t>
+  </si>
+  <si>
+    <t>Sit, in, fin, lid, bit, fix, hip, kit, his, fig, quit, hid, did, hit, gig, pig, lip, fit, if, dim, jig, mix, dip, bin, its, him, lit, fib, pit, blip, clip, disk, lint, mint, flip, slip, drip, fist, slid, grip, slit, brim, swig, limp, sift, slim, gift, tilt, skin, snip, wind, skip, skid, grim, hint, it, win, big, kids, list, trip</t>
+  </si>
+  <si>
+    <t>Bop, jog, job, cot, jot, rot, not, dot, lop, lot, pod, sob, cod, bog, mop, top, fox, log, dog, got, fog, cop, nod, rod, on, hot, hop, box, pop, stop, trot, clot, bond, fond, loft, prod, pond, spot, slob, clog, frog, hogs, logs, moms, mom, crop, cost, dogs, plot, soft, flop, pots, plop, sobs, slot, blot</t>
   </si>
   <si>
     <t>at, is, on, mom, him, job, map, sat, and, man, had, if, sit, his, six, not, got, lot, top, fast, land, spot, wind, fit, kids, stop, hop, skip</t>
@@ -2951,8 +2951,8 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="B16">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5046,7 +5046,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>